<commit_message>
Fixed scaling issues for all images
</commit_message>
<xml_diff>
--- a/Parker Sensor List.xlsx
+++ b/Parker Sensor List.xlsx
@@ -2852,9 +2852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1524000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2872,7 +2872,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9496425" y="3352800"/>
-          <a:ext cx="1524000" cy="1524000"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2909,7 +2909,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="5381625"/>
+          <a:off x="9496425" y="4933950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2947,7 +2947,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="7153275"/>
+          <a:off x="9496425" y="6705600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2985,7 +2985,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="8734425"/>
+          <a:off x="9496425" y="8286750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3023,7 +3023,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="10315575"/>
+          <a:off x="9496425" y="9867900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3061,7 +3061,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="11896725"/>
+          <a:off x="9496425" y="11449050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3099,7 +3099,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="13477875"/>
+          <a:off x="9496425" y="13030200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3137,7 +3137,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="15059025"/>
+          <a:off x="9496425" y="14611350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3175,7 +3175,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="16640175"/>
+          <a:off x="9496425" y="16192500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3213,7 +3213,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="18221325"/>
+          <a:off x="9496425" y="17773650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3251,7 +3251,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="19802475"/>
+          <a:off x="9496425" y="19354800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3289,7 +3289,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="21383625"/>
+          <a:off x="9496425" y="20935950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3327,7 +3327,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="22964775"/>
+          <a:off x="9496425" y="22517100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3365,7 +3365,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="24545925"/>
+          <a:off x="9496425" y="24098250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3403,7 +3403,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="26127075"/>
+          <a:off x="9496425" y="25679400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3422,9 +3422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3441,8 +3441,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="27708225"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="27260550"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3479,7 +3479,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="29441775"/>
+          <a:off x="9496425" y="28841700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3517,7 +3517,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="31022925"/>
+          <a:off x="9496425" y="30422850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3555,7 +3555,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="32604075"/>
+          <a:off x="9496425" y="32004000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3593,7 +3593,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="34185225"/>
+          <a:off x="9496425" y="33585150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3631,7 +3631,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="35766375"/>
+          <a:off x="9496425" y="35166300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3669,7 +3669,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="37347525"/>
+          <a:off x="9496425" y="36747450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3707,7 +3707,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="38928675"/>
+          <a:off x="9496425" y="38328600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3745,7 +3745,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="40509825"/>
+          <a:off x="9496425" y="39909750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3783,7 +3783,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="42090975"/>
+          <a:off x="9496425" y="41490900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3821,7 +3821,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="43672125"/>
+          <a:off x="9496425" y="43072050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3840,9 +3840,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>1524000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3859,8 +3859,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="45253275"/>
-          <a:ext cx="1524000" cy="1524000"/>
+          <a:off x="9496425" y="44653200"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3897,7 +3897,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="47282100"/>
+          <a:off x="9496425" y="46234350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3935,7 +3935,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="48863250"/>
+          <a:off x="9496425" y="47815500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3973,7 +3973,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="50444400"/>
+          <a:off x="9496425" y="49396650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4011,7 +4011,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="52025550"/>
+          <a:off x="9496425" y="50977800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4049,7 +4049,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="53606700"/>
+          <a:off x="9496425" y="52558950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4087,7 +4087,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="55187850"/>
+          <a:off x="9496425" y="54140100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4125,7 +4125,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="56769000"/>
+          <a:off x="9496425" y="55721250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4163,7 +4163,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="58350150"/>
+          <a:off x="9496425" y="57302400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4201,7 +4201,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="59931300"/>
+          <a:off x="9496425" y="58883550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4239,7 +4239,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="61512450"/>
+          <a:off x="9496425" y="60464700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4277,7 +4277,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="63093600"/>
+          <a:off x="9496425" y="62045850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4315,7 +4315,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="64674750"/>
+          <a:off x="9496425" y="63627000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4353,7 +4353,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="66255900"/>
+          <a:off x="9496425" y="65208150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4391,7 +4391,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="67837050"/>
+          <a:off x="9496425" y="66789300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4429,7 +4429,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="69418200"/>
+          <a:off x="9496425" y="68370450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4467,7 +4467,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="70999350"/>
+          <a:off x="9496425" y="69951600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4505,7 +4505,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="72580500"/>
+          <a:off x="9496425" y="71532750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4543,7 +4543,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="74161650"/>
+          <a:off x="9496425" y="73113900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4581,7 +4581,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="75742800"/>
+          <a:off x="9496425" y="74695050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4619,7 +4619,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="77323950"/>
+          <a:off x="9496425" y="76276200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4657,7 +4657,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="78905100"/>
+          <a:off x="9496425" y="77857350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4695,7 +4695,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="80486250"/>
+          <a:off x="9496425" y="79438500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4714,9 +4714,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4733,8 +4733,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="82067400"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="81019650"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4771,7 +4771,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="83591400"/>
+          <a:off x="9496425" y="82600800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4809,7 +4809,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="85172550"/>
+          <a:off x="9496425" y="84181950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4828,9 +4828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4847,8 +4847,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="86753700"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="85763100"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4885,7 +4885,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="88277700"/>
+          <a:off x="9496425" y="87344250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4904,9 +4904,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4923,8 +4923,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="89858850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="88925400"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4942,9 +4942,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4961,8 +4961,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="91382850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="90506550"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4980,9 +4980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4999,8 +4999,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="92906850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="92087700"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5018,9 +5018,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5037,8 +5037,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="94430850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="93668850"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5056,9 +5056,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5075,8 +5075,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="95954850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="95250000"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5094,9 +5094,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5113,8 +5113,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="97478850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="96831150"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5132,9 +5132,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5151,8 +5151,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="99002850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="98412300"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5170,9 +5170,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5189,8 +5189,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="100526850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="99993450"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5208,9 +5208,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5227,8 +5227,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="102050850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="101574600"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5246,9 +5246,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5265,8 +5265,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="103574850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="103155750"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5284,9 +5284,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5303,8 +5303,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="105098850"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="104736900"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5341,7 +5341,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="106622850"/>
+          <a:off x="9496425" y="106318050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5360,9 +5360,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5379,8 +5379,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="108204000"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="107899200"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5398,9 +5398,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5417,8 +5417,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="109937550"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="109480350"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5436,9 +5436,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5455,8 +5455,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="111671100"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="111061500"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5474,9 +5474,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5493,8 +5493,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="113404650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="112642650"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5512,9 +5512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5531,8 +5531,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="114928650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="114223800"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5550,9 +5550,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5569,8 +5569,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="116452650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="115804950"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5588,9 +5588,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5607,8 +5607,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="117976650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="117386100"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5626,9 +5626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5645,8 +5645,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="119500650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="118967250"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5664,9 +5664,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5683,8 +5683,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="121024650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="120548400"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5702,9 +5702,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5721,8 +5721,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="122548650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="122129550"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5740,9 +5740,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5759,8 +5759,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="124072650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="123710700"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5778,9 +5778,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5797,8 +5797,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="125596650"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="125291850"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5835,7 +5835,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="127120650"/>
+          <a:off x="9496425" y="126873000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5873,7 +5873,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="128701800"/>
+          <a:off x="9496425" y="128454150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5911,7 +5911,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="130282950"/>
+          <a:off x="9496425" y="130035300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5949,7 +5949,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="131864100"/>
+          <a:off x="9496425" y="131616450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5987,7 +5987,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="133445250"/>
+          <a:off x="9496425" y="133197600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6025,7 +6025,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="135026400"/>
+          <a:off x="9496425" y="134778750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6063,7 +6063,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="136607550"/>
+          <a:off x="9496425" y="136359900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6101,7 +6101,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="138188700"/>
+          <a:off x="9496425" y="137941050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6139,7 +6139,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="139769850"/>
+          <a:off x="9496425" y="139522200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6158,9 +6158,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6177,8 +6177,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="141351000"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="141103350"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6215,7 +6215,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="143084550"/>
+          <a:off x="9496425" y="142684500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6253,7 +6253,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="144665700"/>
+          <a:off x="9496425" y="144265650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6291,7 +6291,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="146246850"/>
+          <a:off x="9496425" y="145846800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6329,7 +6329,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="147828000"/>
+          <a:off x="9496425" y="147427950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6367,7 +6367,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="149409150"/>
+          <a:off x="9496425" y="149009100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6405,7 +6405,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="150990300"/>
+          <a:off x="9496425" y="150590250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6443,7 +6443,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="152571450"/>
+          <a:off x="9496425" y="152171400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6481,7 +6481,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="154152600"/>
+          <a:off x="9496425" y="153752550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6519,7 +6519,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="155733750"/>
+          <a:off x="9496425" y="155333700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6557,7 +6557,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="157314900"/>
+          <a:off x="9496425" y="156914850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6595,7 +6595,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="158896050"/>
+          <a:off x="9496425" y="158496000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6633,7 +6633,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="160477200"/>
+          <a:off x="9496425" y="160077150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6671,7 +6671,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="162058350"/>
+          <a:off x="9496425" y="161658300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6709,7 +6709,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="163639500"/>
+          <a:off x="9496425" y="163239450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6747,7 +6747,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="165220650"/>
+          <a:off x="9496425" y="164820600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6785,7 +6785,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="166801800"/>
+          <a:off x="9496425" y="166401750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6823,7 +6823,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="168382950"/>
+          <a:off x="9496425" y="167982900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6861,7 +6861,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="169964100"/>
+          <a:off x="9496425" y="169564050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6899,7 +6899,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="171545250"/>
+          <a:off x="9496425" y="171145200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6937,7 +6937,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="173126400"/>
+          <a:off x="9496425" y="172726350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6975,7 +6975,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="174707550"/>
+          <a:off x="9496425" y="174307500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7013,7 +7013,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="176288700"/>
+          <a:off x="9496425" y="175888650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7051,7 +7051,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="177869850"/>
+          <a:off x="9496425" y="177469800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7089,7 +7089,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="179451000"/>
+          <a:off x="9496425" y="179050950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7127,7 +7127,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="181032150"/>
+          <a:off x="9496425" y="180632100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7165,7 +7165,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="182613300"/>
+          <a:off x="9496425" y="182213250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7203,7 +7203,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="184194450"/>
+          <a:off x="9496425" y="183794400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7241,7 +7241,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="185775600"/>
+          <a:off x="9496425" y="185375550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7279,7 +7279,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="187356750"/>
+          <a:off x="9496425" y="186956700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7317,7 +7317,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="188937900"/>
+          <a:off x="9496425" y="188537850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7355,7 +7355,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="190519050"/>
+          <a:off x="9496425" y="190119000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7376,7 +7376,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>123</xdr:row>
-      <xdr:rowOff>1114425</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7393,8 +7393,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="192100200"/>
-          <a:ext cx="1304925" cy="1114425"/>
+          <a:off x="9496425" y="191700150"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7412,9 +7412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7431,8 +7431,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="193586100"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="193281300"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7450,9 +7450,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7469,8 +7469,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="195110100"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="194862450"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7507,7 +7507,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="196634100"/>
+          <a:off x="9496425" y="196443600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7545,7 +7545,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="198215250"/>
+          <a:off x="9496425" y="198024750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7583,7 +7583,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="199796400"/>
+          <a:off x="9496425" y="199605900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7621,7 +7621,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="201377550"/>
+          <a:off x="9496425" y="201187050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7659,7 +7659,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="202958700"/>
+          <a:off x="9496425" y="202768200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7697,7 +7697,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="204539850"/>
+          <a:off x="9496425" y="204349350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7735,7 +7735,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="206121000"/>
+          <a:off x="9496425" y="205930500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7756,7 +7756,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>1209675</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7773,8 +7773,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="207702150"/>
-          <a:ext cx="1304925" cy="1209675"/>
+          <a:off x="9496425" y="207511650"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7811,7 +7811,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="209311875"/>
+          <a:off x="9496425" y="209092800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7849,7 +7849,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="210893025"/>
+          <a:off x="9496425" y="210673950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7887,7 +7887,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="212474175"/>
+          <a:off x="9496425" y="212255100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7925,7 +7925,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="214055325"/>
+          <a:off x="9496425" y="213836250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7963,7 +7963,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="215636475"/>
+          <a:off x="9496425" y="215417400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8001,7 +8001,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="217217625"/>
+          <a:off x="9496425" y="216998550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8039,7 +8039,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="218798775"/>
+          <a:off x="9496425" y="218579700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8077,7 +8077,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="220379925"/>
+          <a:off x="9496425" y="220160850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8115,7 +8115,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="221961075"/>
+          <a:off x="9496425" y="221742000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8153,7 +8153,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="223542225"/>
+          <a:off x="9496425" y="223323150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8191,7 +8191,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="225123375"/>
+          <a:off x="9496425" y="224904300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8229,7 +8229,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="226704525"/>
+          <a:off x="9496425" y="226485450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8267,7 +8267,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="228285675"/>
+          <a:off x="9496425" y="228066600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8305,7 +8305,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="229866825"/>
+          <a:off x="9496425" y="229647750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8343,7 +8343,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="231447975"/>
+          <a:off x="9496425" y="231228900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8381,7 +8381,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="233029125"/>
+          <a:off x="9496425" y="232810050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8419,7 +8419,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="234610275"/>
+          <a:off x="9496425" y="234391200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8457,7 +8457,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="236191425"/>
+          <a:off x="9496425" y="235972350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8495,7 +8495,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="237772575"/>
+          <a:off x="9496425" y="237553500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8533,7 +8533,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="239353725"/>
+          <a:off x="9496425" y="239134650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8571,7 +8571,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="240934875"/>
+          <a:off x="9496425" y="240715800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8609,7 +8609,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="242516025"/>
+          <a:off x="9496425" y="242296950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8647,7 +8647,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="244097175"/>
+          <a:off x="9496425" y="243878100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8685,7 +8685,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="245678325"/>
+          <a:off x="9496425" y="245459250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8723,7 +8723,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="247259475"/>
+          <a:off x="9496425" y="247040400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8761,7 +8761,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="248840625"/>
+          <a:off x="9496425" y="248621550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8780,9 +8780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>160</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8799,8 +8799,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="250421775"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="250202700"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8837,7 +8837,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="251945775"/>
+          <a:off x="9496425" y="251783850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8856,9 +8856,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>162</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8875,8 +8875,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="253526925"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="253365000"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8913,7 +8913,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="255050925"/>
+          <a:off x="9496425" y="254946150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8951,7 +8951,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="256632075"/>
+          <a:off x="9496425" y="256527300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8989,7 +8989,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="258213225"/>
+          <a:off x="9496425" y="258108450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9027,7 +9027,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="259794375"/>
+          <a:off x="9496425" y="259689600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9046,9 +9046,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>167</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9065,8 +9065,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="261375525"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="261270750"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9084,9 +9084,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>168</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9103,8 +9103,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="262899525"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="262851900"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9122,9 +9122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9141,8 +9141,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="264633075"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="264433050"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9160,9 +9160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9179,8 +9179,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="266366625"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="266014200"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9198,9 +9198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>171</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9217,8 +9217,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="268100175"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="267595350"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9236,9 +9236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>172</xdr:row>
-      <xdr:rowOff>819150</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9255,8 +9255,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="269833725"/>
-          <a:ext cx="1143000" cy="819150"/>
+          <a:off x="9496425" y="269176500"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9274,9 +9274,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>173</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9293,8 +9293,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="270919575"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="270757650"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9312,9 +9312,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>174</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9331,8 +9331,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="272653125"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="272338800"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9350,9 +9350,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>175</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9369,8 +9369,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="274386675"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="273919950"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9388,9 +9388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>176</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9407,8 +9407,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="276120225"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="275501100"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9426,9 +9426,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>177</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9445,8 +9445,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="277853775"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="277082250"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9464,9 +9464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>178</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9483,8 +9483,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="279587325"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="278663400"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9502,9 +9502,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>179</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9521,8 +9521,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="281320875"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="280244550"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9540,9 +9540,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>180</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9559,8 +9559,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="282844875"/>
-          <a:ext cx="1333500" cy="1143000"/>
+          <a:off x="9496425" y="281825700"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9578,9 +9578,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9597,8 +9597,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="284368875"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="283406850"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9616,9 +9616,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9635,8 +9635,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="286102425"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="284988000"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9654,9 +9654,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>183</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9673,8 +9673,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="287835975"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="286569150"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9692,9 +9692,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>184</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9711,8 +9711,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="289569525"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="288150300"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9730,9 +9730,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>185</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9749,8 +9749,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="291303075"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="289731450"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9768,9 +9768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>186</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9787,8 +9787,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="293036625"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="291312600"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9806,9 +9806,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9825,8 +9825,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="294770175"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="292893750"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9844,9 +9844,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>188</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9863,8 +9863,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="296503725"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="294474900"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9882,9 +9882,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>189</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9901,8 +9901,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="298237275"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="296056050"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9920,9 +9920,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>190</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9939,8 +9939,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="299970825"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="297637200"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9958,9 +9958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>191</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9977,8 +9977,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="301704375"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="299218350"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9996,9 +9996,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>192</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10015,8 +10015,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="303437925"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="300799500"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10034,9 +10034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>193</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10053,8 +10053,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="305171475"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="302380650"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10072,9 +10072,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>194</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10091,8 +10091,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="306905025"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="303961800"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10110,9 +10110,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>195</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10129,8 +10129,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="308638575"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="305542950"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10148,9 +10148,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>196</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10167,8 +10167,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="310372125"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="307124100"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10205,7 +10205,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="312105675"/>
+          <a:off x="9496425" y="308705250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10224,9 +10224,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>198</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10243,8 +10243,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="313686825"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="310286400"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10281,7 +10281,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="315420375"/>
+          <a:off x="9496425" y="311867550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10319,7 +10319,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="317001525"/>
+          <a:off x="9496425" y="313448700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10357,7 +10357,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="318582675"/>
+          <a:off x="9496425" y="315029850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10395,7 +10395,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="320163825"/>
+          <a:off x="9496425" y="316611000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10433,7 +10433,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="321744975"/>
+          <a:off x="9496425" y="318192150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10471,7 +10471,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="323326125"/>
+          <a:off x="9496425" y="319773300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10509,7 +10509,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="324907275"/>
+          <a:off x="9496425" y="321354450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10547,7 +10547,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="326488425"/>
+          <a:off x="9496425" y="322935600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10585,7 +10585,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="328069575"/>
+          <a:off x="9496425" y="324516750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10623,7 +10623,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="329650725"/>
+          <a:off x="9496425" y="326097900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10661,7 +10661,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="331231875"/>
+          <a:off x="9496425" y="327679050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10699,7 +10699,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="332813025"/>
+          <a:off x="9496425" y="329260200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10737,7 +10737,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="334394175"/>
+          <a:off x="9496425" y="330841350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10775,7 +10775,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="335975325"/>
+          <a:off x="9496425" y="332422500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10813,7 +10813,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="337556475"/>
+          <a:off x="9496425" y="334003650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10851,7 +10851,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="339137625"/>
+          <a:off x="9496425" y="335584800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10889,7 +10889,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="340718775"/>
+          <a:off x="9496425" y="337165950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10927,7 +10927,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="342299925"/>
+          <a:off x="9496425" y="338747100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10965,7 +10965,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="343881075"/>
+          <a:off x="9496425" y="340328250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11003,7 +11003,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="345462225"/>
+          <a:off x="9496425" y="341909400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11041,7 +11041,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="347043375"/>
+          <a:off x="9496425" y="343490550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11079,7 +11079,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="348624525"/>
+          <a:off x="9496425" y="345071700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11117,7 +11117,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="350205675"/>
+          <a:off x="9496425" y="346652850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11155,7 +11155,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="351786825"/>
+          <a:off x="9496425" y="348234000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11193,7 +11193,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="353367975"/>
+          <a:off x="9496425" y="349815150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11231,7 +11231,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="354949125"/>
+          <a:off x="9496425" y="351396300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11269,7 +11269,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="356530275"/>
+          <a:off x="9496425" y="352977450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11307,7 +11307,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="358111425"/>
+          <a:off x="9496425" y="354558600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11345,7 +11345,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="359692575"/>
+          <a:off x="9496425" y="356139750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11383,7 +11383,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="361273725"/>
+          <a:off x="9496425" y="357720900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11421,7 +11421,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="362854875"/>
+          <a:off x="9496425" y="359302050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11440,9 +11440,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>230</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11459,8 +11459,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="364436025"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="360883200"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11478,9 +11478,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>231</xdr:row>
-      <xdr:rowOff>1304925</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11497,8 +11497,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="366169575"/>
-          <a:ext cx="1190625" cy="1304925"/>
+          <a:off x="9496425" y="362464350"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11535,7 +11535,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="367903125"/>
+          <a:off x="9496425" y="364045500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11573,7 +11573,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="369484275"/>
+          <a:off x="9496425" y="365626650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11611,7 +11611,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="371065425"/>
+          <a:off x="9496425" y="367207800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11649,7 +11649,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="372646575"/>
+          <a:off x="9496425" y="368788950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11687,7 +11687,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="374227725"/>
+          <a:off x="9496425" y="370370100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11725,7 +11725,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="375808875"/>
+          <a:off x="9496425" y="371951250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11763,7 +11763,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="377390025"/>
+          <a:off x="9496425" y="373532400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11801,7 +11801,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="378971175"/>
+          <a:off x="9496425" y="375113550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11839,7 +11839,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="380552325"/>
+          <a:off x="9496425" y="376694700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11877,7 +11877,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="382133475"/>
+          <a:off x="9496425" y="378275850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11915,7 +11915,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="383714625"/>
+          <a:off x="9496425" y="379857000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11953,7 +11953,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="385295775"/>
+          <a:off x="9496425" y="381438150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11991,7 +11991,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="386876925"/>
+          <a:off x="9496425" y="383019300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12029,7 +12029,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="388458075"/>
+          <a:off x="9496425" y="384600450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12067,7 +12067,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="390039225"/>
+          <a:off x="9496425" y="386181600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12105,7 +12105,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="391620375"/>
+          <a:off x="9496425" y="387762750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12143,7 +12143,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="393201525"/>
+          <a:off x="9496425" y="389343900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12181,7 +12181,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="394782675"/>
+          <a:off x="9496425" y="390925050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12219,7 +12219,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="396363825"/>
+          <a:off x="9496425" y="392506200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12257,7 +12257,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="397944975"/>
+          <a:off x="9496425" y="394087350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12295,7 +12295,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="399526125"/>
+          <a:off x="9496425" y="395668500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12333,7 +12333,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="401107275"/>
+          <a:off x="9496425" y="397249650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12371,7 +12371,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="402688425"/>
+          <a:off x="9496425" y="398830800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12409,7 +12409,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="404269575"/>
+          <a:off x="9496425" y="400411950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12447,7 +12447,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="405850725"/>
+          <a:off x="9496425" y="401993100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12485,7 +12485,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="407431875"/>
+          <a:off x="9496425" y="403574250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12523,7 +12523,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="409013025"/>
+          <a:off x="9496425" y="405155400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12561,7 +12561,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="410594175"/>
+          <a:off x="9496425" y="406736550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12599,7 +12599,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="412175325"/>
+          <a:off x="9496425" y="408317700"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12637,7 +12637,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="413756475"/>
+          <a:off x="9496425" y="409898850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12675,7 +12675,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="415337625"/>
+          <a:off x="9496425" y="411480000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12713,7 +12713,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="416918775"/>
+          <a:off x="9496425" y="413061150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12751,7 +12751,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="418499925"/>
+          <a:off x="9496425" y="414642300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12789,7 +12789,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="420081075"/>
+          <a:off x="9496425" y="416223450"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12827,7 +12827,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="421662225"/>
+          <a:off x="9496425" y="417804600"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12865,7 +12865,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="423243375"/>
+          <a:off x="9496425" y="419385750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12903,7 +12903,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="424824525"/>
+          <a:off x="9496425" y="420966900"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12941,7 +12941,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="426405675"/>
+          <a:off x="9496425" y="422548050"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12979,7 +12979,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="427986825"/>
+          <a:off x="9496425" y="424129200"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13017,7 +13017,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="429567975"/>
+          <a:off x="9496425" y="425710350"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13055,7 +13055,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="431149125"/>
+          <a:off x="9496425" y="427291500"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13093,7 +13093,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="432730275"/>
+          <a:off x="9496425" y="428872650"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13131,7 +13131,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="434311425"/>
+          <a:off x="9496425" y="430453800"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13169,7 +13169,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="435892575"/>
+          <a:off x="9496425" y="432034950"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13207,7 +13207,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="437473725"/>
+          <a:off x="9496425" y="433616100"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13245,7 +13245,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="439054875"/>
+          <a:off x="9496425" y="435197250"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13283,7 +13283,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="440636025"/>
+          <a:off x="9496425" y="436778400"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13321,7 +13321,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="442217175"/>
+          <a:off x="9496425" y="438359550"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13339,10 +13339,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>280</xdr:row>
-      <xdr:rowOff>9525000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13359,8 +13359,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="443798325"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:off x="9496425" y="439940700"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13397,7 +13397,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="456495150"/>
+          <a:off x="9496425" y="441521850"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13435,7 +13435,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="458076300"/>
+          <a:off x="9496425" y="443103000"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13473,7 +13473,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="459657450"/>
+          <a:off x="9496425" y="444684150"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13511,7 +13511,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="461238600"/>
+          <a:off x="9496425" y="446265300"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13529,10 +13529,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>285</xdr:row>
-      <xdr:rowOff>9525000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13549,8 +13549,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="462819750"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:off x="9496425" y="447846450"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13567,10 +13567,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>286</xdr:row>
-      <xdr:rowOff>9525000</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13587,8 +13587,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="475516575"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:off x="9496425" y="449427600"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13625,7 +13625,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="488213400"/>
+          <a:off x="9496425" y="451008750"/>
           <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13644,9 +13644,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6353175</xdr:colOff>
+      <xdr:colOff>1304925</xdr:colOff>
       <xdr:row>288</xdr:row>
-      <xdr:rowOff>6353175</xdr:rowOff>
+      <xdr:rowOff>1190625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13663,8 +13663,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9496425" y="489794550"/>
-          <a:ext cx="6353175" cy="6353175"/>
+          <a:off x="9496425" y="452589900"/>
+          <a:ext cx="1304925" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13969,7 +13969,7 @@
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="133.7109375" customWidth="1"/>
-    <col min="3" max="3" width="142.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="100.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="133.7109375" customWidth="1"/>
   </cols>
@@ -14019,7 +14019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="160" customHeight="1">
+    <row r="4" spans="1:5" ht="125" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -14246,7 +14246,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="137" customHeight="1">
+    <row r="20" spans="1:5" ht="125" customHeight="1">
       <c r="A20">
         <v>19</v>
       </c>
@@ -14400,7 +14400,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="160" customHeight="1">
+    <row r="31" spans="1:5" ht="125" customHeight="1">
       <c r="A31">
         <v>30</v>
       </c>
@@ -14722,7 +14722,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="120" customHeight="1">
+    <row r="54" spans="1:5" ht="125" customHeight="1">
       <c r="A54">
         <v>53</v>
       </c>
@@ -14764,7 +14764,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="120" customHeight="1">
+    <row r="57" spans="1:5" ht="125" customHeight="1">
       <c r="A57">
         <v>56</v>
       </c>
@@ -14792,7 +14792,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="120" customHeight="1">
+    <row r="59" spans="1:5" ht="125" customHeight="1">
       <c r="A59">
         <v>58</v>
       </c>
@@ -14806,7 +14806,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="120" customHeight="1">
+    <row r="60" spans="1:5" ht="125" customHeight="1">
       <c r="A60">
         <v>59</v>
       </c>
@@ -14820,7 +14820,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="120" customHeight="1">
+    <row r="61" spans="1:5" ht="125" customHeight="1">
       <c r="A61">
         <v>60</v>
       </c>
@@ -14834,7 +14834,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="120" customHeight="1">
+    <row r="62" spans="1:5" ht="125" customHeight="1">
       <c r="A62">
         <v>61</v>
       </c>
@@ -14848,7 +14848,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="120" customHeight="1">
+    <row r="63" spans="1:5" ht="125" customHeight="1">
       <c r="A63">
         <v>62</v>
       </c>
@@ -14862,7 +14862,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="120" customHeight="1">
+    <row r="64" spans="1:5" ht="125" customHeight="1">
       <c r="A64">
         <v>63</v>
       </c>
@@ -14876,7 +14876,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="120" customHeight="1">
+    <row r="65" spans="1:5" ht="125" customHeight="1">
       <c r="A65">
         <v>64</v>
       </c>
@@ -14890,7 +14890,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="120" customHeight="1">
+    <row r="66" spans="1:5" ht="125" customHeight="1">
       <c r="A66">
         <v>65</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="120" customHeight="1">
+    <row r="67" spans="1:5" ht="125" customHeight="1">
       <c r="A67">
         <v>66</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="120" customHeight="1">
+    <row r="68" spans="1:5" ht="125" customHeight="1">
       <c r="A68">
         <v>67</v>
       </c>
@@ -14932,7 +14932,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="120" customHeight="1">
+    <row r="69" spans="1:5" ht="125" customHeight="1">
       <c r="A69">
         <v>68</v>
       </c>
@@ -14960,7 +14960,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="137" customHeight="1">
+    <row r="71" spans="1:5" ht="125" customHeight="1">
       <c r="A71">
         <v>70</v>
       </c>
@@ -14974,7 +14974,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="137" customHeight="1">
+    <row r="72" spans="1:5" ht="125" customHeight="1">
       <c r="A72">
         <v>71</v>
       </c>
@@ -14988,7 +14988,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="137" customHeight="1">
+    <row r="73" spans="1:5" ht="125" customHeight="1">
       <c r="A73">
         <v>72</v>
       </c>
@@ -15002,7 +15002,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="120" customHeight="1">
+    <row r="74" spans="1:5" ht="125" customHeight="1">
       <c r="A74">
         <v>73</v>
       </c>
@@ -15016,7 +15016,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="120" customHeight="1">
+    <row r="75" spans="1:5" ht="125" customHeight="1">
       <c r="A75">
         <v>74</v>
       </c>
@@ -15030,7 +15030,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="120" customHeight="1">
+    <row r="76" spans="1:5" ht="125" customHeight="1">
       <c r="A76">
         <v>75</v>
       </c>
@@ -15044,7 +15044,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="120" customHeight="1">
+    <row r="77" spans="1:5" ht="125" customHeight="1">
       <c r="A77">
         <v>76</v>
       </c>
@@ -15058,7 +15058,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="120" customHeight="1">
+    <row r="78" spans="1:5" ht="125" customHeight="1">
       <c r="A78">
         <v>77</v>
       </c>
@@ -15072,7 +15072,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="120" customHeight="1">
+    <row r="79" spans="1:5" ht="125" customHeight="1">
       <c r="A79">
         <v>78</v>
       </c>
@@ -15086,7 +15086,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="120" customHeight="1">
+    <row r="80" spans="1:5" ht="125" customHeight="1">
       <c r="A80">
         <v>79</v>
       </c>
@@ -15100,7 +15100,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="120" customHeight="1">
+    <row r="81" spans="1:5" ht="125" customHeight="1">
       <c r="A81">
         <v>80</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="120" customHeight="1">
+    <row r="82" spans="1:5" ht="125" customHeight="1">
       <c r="A82">
         <v>81</v>
       </c>
@@ -15254,7 +15254,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="137" customHeight="1">
+    <row r="92" spans="1:5" ht="125" customHeight="1">
       <c r="A92">
         <v>91</v>
       </c>
@@ -15702,7 +15702,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="117" customHeight="1">
+    <row r="124" spans="1:5" ht="125" customHeight="1">
       <c r="A124">
         <v>123</v>
       </c>
@@ -15716,7 +15716,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="120" customHeight="1">
+    <row r="125" spans="1:5" ht="125" customHeight="1">
       <c r="A125">
         <v>124</v>
       </c>
@@ -15730,7 +15730,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="120" customHeight="1">
+    <row r="126" spans="1:5" ht="125" customHeight="1">
       <c r="A126">
         <v>125</v>
       </c>
@@ -15842,7 +15842,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="127" customHeight="1">
+    <row r="134" spans="1:5" ht="125" customHeight="1">
       <c r="A134">
         <v>133</v>
       </c>
@@ -16220,7 +16220,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="120" customHeight="1">
+    <row r="161" spans="1:5" ht="125" customHeight="1">
       <c r="A161">
         <v>160</v>
       </c>
@@ -16248,7 +16248,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="120" customHeight="1">
+    <row r="163" spans="1:5" ht="125" customHeight="1">
       <c r="A163">
         <v>162</v>
       </c>
@@ -16318,7 +16318,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="120" customHeight="1">
+    <row r="168" spans="1:5" ht="125" customHeight="1">
       <c r="A168">
         <v>167</v>
       </c>
@@ -16332,7 +16332,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="137" customHeight="1">
+    <row r="169" spans="1:5" ht="125" customHeight="1">
       <c r="A169">
         <v>168</v>
       </c>
@@ -16346,7 +16346,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="137" customHeight="1">
+    <row r="170" spans="1:5" ht="125" customHeight="1">
       <c r="A170">
         <v>169</v>
       </c>
@@ -16360,7 +16360,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="137" customHeight="1">
+    <row r="171" spans="1:5" ht="125" customHeight="1">
       <c r="A171">
         <v>170</v>
       </c>
@@ -16374,7 +16374,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="137" customHeight="1">
+    <row r="172" spans="1:5" ht="125" customHeight="1">
       <c r="A172">
         <v>171</v>
       </c>
@@ -16388,7 +16388,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="86" customHeight="1">
+    <row r="173" spans="1:5" ht="125" customHeight="1">
       <c r="A173">
         <v>172</v>
       </c>
@@ -16402,7 +16402,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="137" customHeight="1">
+    <row r="174" spans="1:5" ht="125" customHeight="1">
       <c r="A174">
         <v>173</v>
       </c>
@@ -16416,7 +16416,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="137" customHeight="1">
+    <row r="175" spans="1:5" ht="125" customHeight="1">
       <c r="A175">
         <v>174</v>
       </c>
@@ -16430,7 +16430,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="137" customHeight="1">
+    <row r="176" spans="1:5" ht="125" customHeight="1">
       <c r="A176">
         <v>175</v>
       </c>
@@ -16444,7 +16444,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="137" customHeight="1">
+    <row r="177" spans="1:5" ht="125" customHeight="1">
       <c r="A177">
         <v>176</v>
       </c>
@@ -16458,7 +16458,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="137" customHeight="1">
+    <row r="178" spans="1:5" ht="125" customHeight="1">
       <c r="A178">
         <v>177</v>
       </c>
@@ -16472,7 +16472,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="137" customHeight="1">
+    <row r="179" spans="1:5" ht="125" customHeight="1">
       <c r="A179">
         <v>178</v>
       </c>
@@ -16486,7 +16486,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="120" customHeight="1">
+    <row r="180" spans="1:5" ht="125" customHeight="1">
       <c r="A180">
         <v>179</v>
       </c>
@@ -16500,7 +16500,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="120" customHeight="1">
+    <row r="181" spans="1:5" ht="125" customHeight="1">
       <c r="A181">
         <v>180</v>
       </c>
@@ -16514,7 +16514,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="137" customHeight="1">
+    <row r="182" spans="1:5" ht="125" customHeight="1">
       <c r="A182">
         <v>181</v>
       </c>
@@ -16528,7 +16528,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="137" customHeight="1">
+    <row r="183" spans="1:5" ht="125" customHeight="1">
       <c r="A183">
         <v>182</v>
       </c>
@@ -16542,7 +16542,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="137" customHeight="1">
+    <row r="184" spans="1:5" ht="125" customHeight="1">
       <c r="A184">
         <v>183</v>
       </c>
@@ -16556,7 +16556,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="137" customHeight="1">
+    <row r="185" spans="1:5" ht="125" customHeight="1">
       <c r="A185">
         <v>184</v>
       </c>
@@ -16570,7 +16570,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="137" customHeight="1">
+    <row r="186" spans="1:5" ht="125" customHeight="1">
       <c r="A186">
         <v>185</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="137" customHeight="1">
+    <row r="187" spans="1:5" ht="125" customHeight="1">
       <c r="A187">
         <v>186</v>
       </c>
@@ -16598,7 +16598,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="137" customHeight="1">
+    <row r="188" spans="1:5" ht="125" customHeight="1">
       <c r="A188">
         <v>187</v>
       </c>
@@ -16612,7 +16612,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="137" customHeight="1">
+    <row r="189" spans="1:5" ht="125" customHeight="1">
       <c r="A189">
         <v>188</v>
       </c>
@@ -16626,7 +16626,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="137" customHeight="1">
+    <row r="190" spans="1:5" ht="125" customHeight="1">
       <c r="A190">
         <v>189</v>
       </c>
@@ -16640,7 +16640,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="137" customHeight="1">
+    <row r="191" spans="1:5" ht="125" customHeight="1">
       <c r="A191">
         <v>190</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="137" customHeight="1">
+    <row r="192" spans="1:5" ht="125" customHeight="1">
       <c r="A192">
         <v>191</v>
       </c>
@@ -16668,7 +16668,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="137" customHeight="1">
+    <row r="193" spans="1:5" ht="125" customHeight="1">
       <c r="A193">
         <v>192</v>
       </c>
@@ -16682,7 +16682,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="137" customHeight="1">
+    <row r="194" spans="1:5" ht="125" customHeight="1">
       <c r="A194">
         <v>193</v>
       </c>
@@ -16696,7 +16696,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="137" customHeight="1">
+    <row r="195" spans="1:5" ht="125" customHeight="1">
       <c r="A195">
         <v>194</v>
       </c>
@@ -16710,7 +16710,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="137" customHeight="1">
+    <row r="196" spans="1:5" ht="125" customHeight="1">
       <c r="A196">
         <v>195</v>
       </c>
@@ -16724,7 +16724,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="137" customHeight="1">
+    <row r="197" spans="1:5" ht="125" customHeight="1">
       <c r="A197">
         <v>196</v>
       </c>
@@ -16752,7 +16752,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="137" customHeight="1">
+    <row r="199" spans="1:5" ht="125" customHeight="1">
       <c r="A199">
         <v>198</v>
       </c>
@@ -17200,7 +17200,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="137" customHeight="1">
+    <row r="231" spans="1:5" ht="125" customHeight="1">
       <c r="A231">
         <v>230</v>
       </c>
@@ -17214,7 +17214,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="137" customHeight="1">
+    <row r="232" spans="1:5" ht="125" customHeight="1">
       <c r="A232">
         <v>231</v>
       </c>
@@ -17900,7 +17900,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="281" spans="1:5" ht="1000" customHeight="1">
+    <row r="281" spans="1:5" ht="125" customHeight="1">
       <c r="A281">
         <v>280</v>
       </c>
@@ -17970,7 +17970,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="1000" customHeight="1">
+    <row r="286" spans="1:5" ht="125" customHeight="1">
       <c r="A286">
         <v>285</v>
       </c>
@@ -17984,7 +17984,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="287" spans="1:5" ht="1000" customHeight="1">
+    <row r="287" spans="1:5" ht="125" customHeight="1">
       <c r="A287">
         <v>286</v>
       </c>
@@ -18012,7 +18012,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="289" spans="1:5" ht="667" customHeight="1">
+    <row r="289" spans="1:5" ht="125" customHeight="1">
       <c r="A289">
         <v>288</v>
       </c>

</xml_diff>